<commit_message>
Patch bug at siswa gender when exporting to PDF.
</commit_message>
<xml_diff>
--- a/media/excel/Export Siswa.xlsx
+++ b/media/excel/Export Siswa.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,7 +543,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>Wanita</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>Pria</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>Wanita</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -718,6 +718,81 @@
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ilham Shiddiq</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0024633245</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>181113836</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>shdqillham123@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Cimahi</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2003-07-03</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Pria</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Islam</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Padasuka</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>SMK1</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Secret</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Secret</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Secret</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>12 RPL A</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix error when trying to export data siswa into excel while siswa is empty.
</commit_message>
<xml_diff>
--- a/media/excel/Export Siswa.xlsx
+++ b/media/excel/Export Siswa.xlsx
@@ -577,7 +577,7 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>12 RPL A</t>
+          <t>12 A</t>
         </is>
       </c>
     </row>
@@ -646,11 +646,7 @@
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>12 RPL A</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -790,7 +786,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>12 RPL A</t>
+          <t>12 A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve frontend design by using website template
The template are beautifully created by @puikinsh at Colorlib.
</commit_message>
<xml_diff>
--- a/media/excel/Export Siswa.xlsx
+++ b/media/excel/Export Siswa.xlsx
@@ -577,7 +577,7 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>12 A</t>
+          <t>12 RPL A</t>
         </is>
       </c>
     </row>
@@ -646,7 +646,11 @@
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>12 Mekatronika A</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -713,7 +717,11 @@
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>12 Mekatronika A</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -786,7 +794,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>12 A</t>
+          <t>12 RPL A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Improve frontend design by using website template"
This reverts commit c7778bba13348fd052454911ac000dbebf6d05d7.
</commit_message>
<xml_diff>
--- a/media/excel/Export Siswa.xlsx
+++ b/media/excel/Export Siswa.xlsx
@@ -577,7 +577,7 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>12 RPL A</t>
+          <t>12 A</t>
         </is>
       </c>
     </row>
@@ -646,11 +646,7 @@
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>12 Mekatronika A</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -717,11 +713,7 @@
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>12 Mekatronika A</t>
-        </is>
-      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -794,7 +786,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>12 RPL A</t>
+          <t>12 A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish MataPelajaran CRUD view
</commit_message>
<xml_diff>
--- a/media/excel/Export Siswa.xlsx
+++ b/media/excel/Export Siswa.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,37 +513,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Siswa 1</t>
+          <t>Hariz Sufyan Munawar</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0030000001</t>
+          <t>0040172372</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>181110001</t>
+          <t>123213</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>siswa1@gmail.com</t>
+          <t>munawarhariz@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Cimahi</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2003-02-10</t>
+          <t>2021-03-08</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Wanita</t>
+          <t>Pria</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -553,12 +553,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Rumah Siswa 1</t>
+          <t>Lembah Teratai Blok N no.12</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>SMPN 1 Cimahi</t>
+          <t>SMP Negeri 3 Cimahi</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -566,12 +566,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Ayah 1</t>
+          <t>Moch. Yusuf</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Ibu 1</t>
+          <t>Zulaekah</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
@@ -584,22 +584,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Siswa 2</t>
+          <t>Shaddam Amru</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0040000002</t>
+          <t>0031068496</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>181110002</t>
+          <t>123213512</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>siswa2@gmail.com</t>
+          <t>shaddam.a.h@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2004-01-12</t>
+          <t>2021-03-10</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -624,12 +624,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Rumah Siswa 2</t>
+          <t>Cijerah</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>SMPN 2 Cimahi</t>
+          <t>SMP Negeri 4 Bandung</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -637,70 +637,66 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Ayah 2</t>
+          <t>Amri Hasibuan</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Ibu 2</t>
+          <t>Ani Hasibuan</t>
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>12 Mekatronika A</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Siswa 3</t>
+          <t>Ilham Shiddiq</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0030000003</t>
+          <t>0024633245</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>181110003</t>
+          <t>181113836</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>siswa3@gmail.com</t>
+          <t>shdqillham123@gmail.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jakarta</t>
+          <t>Cimahi</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2003-09-24</t>
+          <t>2003-07-03</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Wanita</t>
+          <t>Pria</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Kristen</t>
+          <t>Islam</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Rumah Siswa 3</t>
+          <t>Padasuka</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>SMPN 3 Cimahi</t>
+          <t>SMK1</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -708,95 +704,20 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Ayah 3</t>
+          <t>Secret</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Ibu 3</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>12 Mekatronika A</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Ilham Shiddiq</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0024633245</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>181113836</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>shdqillham123@gmail.com</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Cimahi</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2003-07-03</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Pria</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Islam</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Padasuka</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>SMK1</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>10</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>Secret</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Secret</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>12 RPL A</t>
-        </is>
-      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>